<commit_message>
Inclusao de Codigo MD5 e Diagrama de sequencia
</commit_message>
<xml_diff>
--- a/Time_1/Protocolo/Protocolo.xlsx
+++ b/Time_1/Protocolo/Protocolo.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Procoloco Padrao" sheetId="1" r:id="rId1"/>
     <sheet name="Exemplo" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Diagrama de Sequencia" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
   <si>
     <t>E</t>
   </si>
@@ -148,13 +148,136 @@
   </si>
   <si>
     <t>Exemplo 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comando para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>virar a esquerda</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> em </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF33CC33"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45 graus</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> em </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>running</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> em velocidade média</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comando para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>levantar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>realizado</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> em velocidade baixa</t>
+    </r>
+  </si>
+  <si>
+    <t>WT - Em espera (Waiting)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +301,30 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF33CC33"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,14 +472,991 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CC33"/>
       <color rgb="FF008000"/>
-      <color rgb="FF33CC33"/>
       <color rgb="FF99FF99"/>
       <color rgb="FF99FF66"/>
       <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Elipse 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2903220" y="1950720"/>
+          <a:ext cx="1043940" cy="967740"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Courier New" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Waiting</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Elipse 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5501640" y="1905000"/>
+          <a:ext cx="1043940" cy="967740"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Courier New" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Run</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Elipse 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8389620" y="1912620"/>
+          <a:ext cx="1043940" cy="967740"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Courier New" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Done</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Elipse 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5501640" y="3840480"/>
+          <a:ext cx="1043940" cy="967740"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Courier New" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Fail</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>136678</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>35042</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>168122</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>80762</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector em curva 6"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="7"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="4701540" y="1139460"/>
+          <a:ext cx="45720" cy="1860244"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 909978"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>296698</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>35042</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>8102</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>42662</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Conector em curva 9"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="7"/>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="7463790" y="975630"/>
+          <a:ext cx="7620" cy="2149804"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -4859869"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>462280</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector em curva 12"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="5" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6545580" y="2388870"/>
+          <a:ext cx="12700" cy="1935480"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1800000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Elipse 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11544300" y="1882140"/>
+          <a:ext cx="1043940" cy="967740"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Courier New" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Waiting</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Elipse 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8442960" y="3817620"/>
+          <a:ext cx="1043940" cy="967740"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Courier New" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Waiting</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>296698</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>71638</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>61442</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>94498</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector em curva 22"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="5"/>
+          <a:endCxn id="22" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="7482840" y="3553496"/>
+          <a:ext cx="22860" cy="2203144"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -1619956"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>136678</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114782</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>42662</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Conector em curva 25"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="7"/>
+          <a:endCxn id="21" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="10473690" y="830850"/>
+          <a:ext cx="30480" cy="2416504"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1314967"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:tailEnd type="stealth" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="924997" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="CaixaDeTexto 29"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4328160" y="1249680"/>
+          <a:ext cx="924997" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Mensagem 1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="924997" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="CaixaDeTexto 30"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6926580" y="1242060"/>
+          <a:ext cx="924997" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Mensagem 2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="924997" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="CaixaDeTexto 31"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9951720" y="1242060"/>
+          <a:ext cx="924997" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Mensagem 3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="924997" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="CaixaDeTexto 35"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4396740" y="1943100"/>
+          <a:ext cx="924997" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Mensagem 1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="924997" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="CaixaDeTexto 36"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6850380" y="3124200"/>
+          <a:ext cx="924997" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Mensagem 2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="924997" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="CaixaDeTexto 37"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7094220" y="4617720"/>
+          <a:ext cx="924997" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Mensagem 3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -620,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:AX34"/>
+  <dimension ref="C4:AX35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+      <selection activeCell="BB26" sqref="BB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.21875" defaultRowHeight="14.4"/>
@@ -976,6 +2100,12 @@
       <c r="AE8" s="13"/>
       <c r="AF8" s="13"/>
       <c r="AG8" s="11"/>
+      <c r="AH8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI8" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="3:50">
       <c r="C9" s="6"/>
@@ -1132,18 +2262,24 @@
       </c>
     </row>
     <row r="31" spans="3:4">
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" spans="3:4">
-      <c r="C32" s="4"/>
-      <c r="D32" s="2" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" s="4"/>
+      <c r="D33" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="3:4">
-      <c r="C34" s="15"/>
-      <c r="D34" s="2" t="s">
+    <row r="35" spans="3:4">
+      <c r="C35" s="15"/>
+      <c r="D35" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1157,8 +2293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:BZ15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:BY8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.21875" defaultRowHeight="14.4"/>
@@ -1616,6 +2752,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:78">
+      <c r="A5" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="8" spans="1:78">
       <c r="A8" t="s">
         <v>43</v>
@@ -1844,6 +2985,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:78">
+      <c r="A9" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="14" spans="1:78">
       <c r="AG14" s="16"/>
     </row>
@@ -1852,7 +2998,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1860,11 +3006,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Acrescentado as informacoes das variaveis do Scade
</commit_message>
<xml_diff>
--- a/Time_1/Protocolo/Protocolo.xlsx
+++ b/Time_1/Protocolo/Protocolo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="71">
   <si>
     <t>E</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>RH - Virar a Direita (Right)</t>
-  </si>
-  <si>
-    <t>1 ~ 9 - Intensidade (1 Devagar ~ 9 Rápido)</t>
   </si>
   <si>
     <t>Byte reservado</t>
@@ -216,9 +213,6 @@
   </si>
   <si>
     <t>WT - Em espera (Waiting)</t>
-  </si>
-  <si>
-    <t>Cabeçalho (Header)</t>
   </si>
   <si>
     <t>Informação Complementar (Ex. Rotação em graus, qtd de passos, outros)</t>
@@ -564,12 +558,54 @@
   <si>
     <t>f</t>
   </si>
+  <si>
+    <t>1 ~ 9 - Intensidade/Magnitude (1 Devagar ~ 9 Rápido)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cabeçalho (Header) </t>
+  </si>
+  <si>
+    <t>P_HEADER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P_TOPIC</t>
+  </si>
+  <si>
+    <t>P_FROM</t>
+  </si>
+  <si>
+    <t>P_TO</t>
+  </si>
+  <si>
+    <t>P_CMD</t>
+  </si>
+  <si>
+    <t>P_MAGNITUDE</t>
+  </si>
+  <si>
+    <t>P_CMD_PLUS</t>
+  </si>
+  <si>
+    <t>P_RESERVED</t>
+  </si>
+  <si>
+    <t>P_STATUS</t>
+  </si>
+  <si>
+    <t>P_TIME</t>
+  </si>
+  <si>
+    <t>P_MD5</t>
+  </si>
+  <si>
+    <t>P_TOTAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,8 +657,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -695,6 +738,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -705,10 +753,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -756,8 +805,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutra" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2036,546 +2095,733 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:AX35"/>
+  <dimension ref="F1:BB35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="AW5" sqref="G5:AW5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.21875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="4.21875" style="1"/>
+    <col min="1" max="5" width="4.21875" style="1"/>
+    <col min="6" max="6" width="4.21875" style="17"/>
+    <col min="7" max="16384" width="4.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:50">
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1">
+    <row r="1" spans="6:54">
+      <c r="AE1" s="19">
+        <v>9</v>
+      </c>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+    </row>
+    <row r="2" spans="6:54">
+      <c r="G2" s="18">
+        <v>43</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="18"/>
+      <c r="AR2" s="18"/>
+      <c r="AS2" s="18"/>
+      <c r="AT2" s="18"/>
+      <c r="AU2" s="18"/>
+      <c r="AV2" s="18"/>
+      <c r="AW2" s="18"/>
+    </row>
+    <row r="3" spans="6:54">
+      <c r="G3" s="18">
+        <v>6</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18">
+        <v>6</v>
+      </c>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18">
+        <v>6</v>
+      </c>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="18">
         <v>3</v>
       </c>
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM3" s="18"/>
+      <c r="AN3" s="18">
+        <v>10</v>
+      </c>
+      <c r="AO3" s="18"/>
+      <c r="AP3" s="18"/>
+      <c r="AQ3" s="18"/>
+      <c r="AR3" s="18"/>
+      <c r="AS3" s="18"/>
+      <c r="AT3" s="18"/>
+      <c r="AU3" s="18"/>
+      <c r="AV3" s="18"/>
+      <c r="AW3" s="18"/>
+      <c r="AX3" s="18">
+        <v>32</v>
+      </c>
+      <c r="AY3" s="18"/>
+      <c r="AZ3" s="18"/>
+      <c r="BA3" s="18"/>
+      <c r="BB3" s="18"/>
+    </row>
+    <row r="4" spans="6:54">
       <c r="G4" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1">
         <v>6</v>
       </c>
-      <c r="J4" s="1">
+      <c r="N4" s="1">
         <v>7</v>
       </c>
-      <c r="K4" s="1">
-        <v>8</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="O4" s="1">
+        <v>8</v>
+      </c>
+      <c r="P4" s="1">
         <v>9</v>
       </c>
-      <c r="M4" s="1">
+      <c r="Q4" s="1">
         <v>10</v>
       </c>
-      <c r="N4" s="1">
+      <c r="R4" s="1">
         <v>11</v>
       </c>
-      <c r="O4" s="1">
+      <c r="S4" s="1">
         <v>12</v>
       </c>
-      <c r="P4" s="1">
+      <c r="T4" s="1">
         <v>13</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="U4" s="1">
         <v>14</v>
       </c>
-      <c r="R4" s="1">
+      <c r="V4" s="1">
         <v>15</v>
       </c>
-      <c r="S4" s="1">
+      <c r="W4" s="1">
         <v>16</v>
       </c>
-      <c r="T4" s="1">
+      <c r="X4" s="1">
         <v>17</v>
       </c>
-      <c r="U4" s="1">
+      <c r="Y4" s="1">
         <v>18</v>
       </c>
-      <c r="V4" s="1">
+      <c r="Z4" s="1">
         <v>19</v>
       </c>
-      <c r="W4" s="1">
+      <c r="AA4" s="1">
         <v>20</v>
       </c>
-      <c r="X4" s="1">
+      <c r="AB4" s="1">
         <v>21</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="AC4" s="1">
         <v>22</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AD4" s="1">
         <v>23</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AE4" s="1">
         <v>24</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AF4" s="1">
         <v>25</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AG4" s="1">
         <v>26</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AH4" s="1">
         <v>27</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AI4" s="1">
         <v>28</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AJ4" s="1">
         <v>29</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AK4" s="1">
         <v>30</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AL4" s="1">
         <v>31</v>
       </c>
-      <c r="AI4" s="1">
+      <c r="AM4" s="1">
         <v>32</v>
       </c>
-      <c r="AJ4" s="1">
+      <c r="AN4" s="1">
         <v>33</v>
       </c>
-      <c r="AK4" s="1">
+      <c r="AO4" s="1">
         <v>34</v>
       </c>
-      <c r="AL4" s="1">
+      <c r="AP4" s="1">
         <v>35</v>
       </c>
-      <c r="AM4" s="1">
+      <c r="AQ4" s="1">
         <v>36</v>
       </c>
-      <c r="AN4" s="1">
+      <c r="AR4" s="1">
         <v>37</v>
       </c>
-      <c r="AO4" s="1">
+      <c r="AS4" s="1">
         <v>38</v>
       </c>
-      <c r="AP4" s="1">
+      <c r="AT4" s="1">
         <v>39</v>
       </c>
-      <c r="AQ4" s="1">
+      <c r="AU4" s="1">
         <v>40</v>
       </c>
-      <c r="AR4" s="1">
+      <c r="AV4" s="1">
         <v>41</v>
       </c>
-      <c r="AS4" s="1">
+      <c r="AW4" s="1">
         <v>42</v>
       </c>
-      <c r="AT4" s="1">
+      <c r="AX4" s="1">
         <v>43</v>
       </c>
-      <c r="AU4" s="1">
+      <c r="AY4" s="1">
         <v>44</v>
       </c>
-      <c r="AV4" s="1" t="s">
+      <c r="AZ4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BA4" s="1">
+        <v>73</v>
+      </c>
+      <c r="BB4" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="6:54">
+      <c r="F5" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6">
+        <v>1</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="V5" s="8">
+        <v>0</v>
+      </c>
+      <c r="W5" s="8">
+        <v>0</v>
+      </c>
+      <c r="X5" s="8">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="12">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="3">
+        <v>5</v>
+      </c>
+      <c r="AP5" s="3">
+        <v>4</v>
+      </c>
+      <c r="AQ5" s="3">
+        <v>2</v>
+      </c>
+      <c r="AR5" s="3">
+        <v>3</v>
+      </c>
+      <c r="AS5" s="3">
+        <v>6</v>
+      </c>
+      <c r="AT5" s="3">
+        <v>8</v>
+      </c>
+      <c r="AU5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="3">
+        <v>2</v>
+      </c>
+      <c r="AW5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY5" s="15">
+        <v>5</v>
+      </c>
+      <c r="AZ5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BA5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB5" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="6:54">
+      <c r="AE6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG6" s="12">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="6:54">
+      <c r="F7" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="6:54">
+      <c r="H8" s="2"/>
+      <c r="AE8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG8" s="12">
+        <v>4</v>
+      </c>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="6:54">
+      <c r="F9" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG9" s="12">
+        <v>5</v>
+      </c>
+      <c r="AH9" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="13">
+        <v>4</v>
+      </c>
+      <c r="AJ9" s="13">
+        <v>5</v>
+      </c>
+      <c r="AK9" s="11"/>
+    </row>
+    <row r="10" spans="6:54">
+      <c r="H10" s="2"/>
+      <c r="AE10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG10" s="12">
+        <v>6</v>
+      </c>
+      <c r="AH10" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="13">
+        <v>3</v>
+      </c>
+      <c r="AJ10" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="11"/>
+    </row>
+    <row r="11" spans="6:54">
+      <c r="F11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="6:54">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="U12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="6:54">
+      <c r="F13" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="6:54">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="6:54">
+      <c r="F15" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="6:54">
+      <c r="G16" s="14"/>
+      <c r="H16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8">
+      <c r="G17" s="14"/>
+      <c r="H17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8">
+      <c r="G18" s="14"/>
+      <c r="H18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8">
+      <c r="G19" s="14"/>
+      <c r="H19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8">
+      <c r="G20" s="14"/>
+      <c r="H20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="6:8">
+      <c r="F22" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="6:8">
+      <c r="F24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="6:8">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="6:8">
+      <c r="F26" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="6:8">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="6:8">
+      <c r="F28" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="6:8">
+      <c r="G29" s="7"/>
+      <c r="H29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="6:8">
+      <c r="G30" s="7"/>
+      <c r="H30" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="6:8">
+      <c r="G31" s="7"/>
+      <c r="H31" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="6:8">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="6:8">
+      <c r="F33" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8">
+      <c r="F35" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="AW4" s="1">
-        <v>73</v>
-      </c>
-      <c r="AX4" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="3:50">
-      <c r="C5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" s="8">
-        <v>0</v>
-      </c>
-      <c r="S5" s="8">
-        <v>0</v>
-      </c>
-      <c r="T5" s="8">
-        <v>1</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="V5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="X5" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC5" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ5" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="3">
-        <v>5</v>
-      </c>
-      <c r="AL5" s="3">
-        <v>4</v>
-      </c>
-      <c r="AM5" s="3">
-        <v>2</v>
-      </c>
-      <c r="AN5" s="3">
-        <v>3</v>
-      </c>
-      <c r="AO5" s="3">
-        <v>6</v>
-      </c>
-      <c r="AP5" s="3">
-        <v>8</v>
-      </c>
-      <c r="AQ5" s="3">
-        <v>1</v>
-      </c>
-      <c r="AR5" s="3">
-        <v>2</v>
-      </c>
-      <c r="AS5" s="3">
-        <v>1</v>
-      </c>
-      <c r="AT5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="AU5" s="15">
-        <v>5</v>
-      </c>
-      <c r="AV5" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX5" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="3:50">
-      <c r="AA6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC6" s="12">
-        <v>2</v>
-      </c>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="3:50">
-      <c r="C7" s="10"/>
-      <c r="D7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC7" s="12">
-        <v>3</v>
-      </c>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="11"/>
-      <c r="AH7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI7" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="3:50">
-      <c r="D8" s="2"/>
-      <c r="AA8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC8" s="12">
-        <v>4</v>
-      </c>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AI8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="3:50">
-      <c r="C9" s="6"/>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB9" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC9" s="12">
-        <v>5</v>
-      </c>
-      <c r="AD9" s="13">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="13">
-        <v>4</v>
-      </c>
-      <c r="AF9" s="13">
-        <v>5</v>
-      </c>
-      <c r="AG9" s="11"/>
-    </row>
-    <row r="10" spans="3:50">
-      <c r="D10" s="2"/>
-      <c r="AA10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC10" s="12">
-        <v>6</v>
-      </c>
-      <c r="AD10" s="13">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="13">
-        <v>3</v>
-      </c>
-      <c r="AF10" s="13">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="11"/>
-    </row>
-    <row r="11" spans="3:50">
-      <c r="C11" s="8"/>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AS11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="3:50">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="3:50">
-      <c r="C13" s="9"/>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="3:50">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="3:50">
-      <c r="C15" s="14"/>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="3:50">
-      <c r="C16" s="14"/>
-      <c r="D16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="C17" s="14"/>
-      <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18" s="14"/>
-      <c r="D18" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4">
-      <c r="C19" s="14"/>
-      <c r="D19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4">
-      <c r="C20" s="14"/>
-      <c r="D20" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="3:4">
-      <c r="C22" s="12"/>
-      <c r="D22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="3:4">
-      <c r="C24" s="13"/>
-      <c r="D24" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4">
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="3:4">
-      <c r="C26" s="11"/>
-      <c r="D26" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4">
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="3:4">
-      <c r="C28" s="7"/>
-      <c r="D28" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4">
-      <c r="C29" s="7"/>
-      <c r="D29" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4">
-      <c r="C30" s="7"/>
-      <c r="D30" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4">
-      <c r="C31" s="7"/>
-      <c r="D31" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="3:4">
-      <c r="C33" s="4"/>
-      <c r="D33" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4">
-      <c r="C35" s="15"/>
-      <c r="D35" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AN3:AW3"/>
+    <mergeCell ref="G2:AW2"/>
+    <mergeCell ref="AE1:AM1"/>
+    <mergeCell ref="AX3:BB3"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="S3:X3"/>
+    <mergeCell ref="Y3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AH3:AJ3"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2825,15 +3071,15 @@
     </row>
     <row r="4" spans="1:79">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:79">
       <c r="A5" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>3</v>
@@ -3013,22 +3259,22 @@
         <v>1</v>
       </c>
       <c r="BK5" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BL5" s="15">
         <v>9</v>
       </c>
       <c r="BM5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BN5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="BN5" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="BO5" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BP5" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BQ5" s="15">
         <v>0</v>
@@ -3037,13 +3283,13 @@
         <v>5</v>
       </c>
       <c r="BS5" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BT5" s="15">
         <v>9</v>
       </c>
       <c r="BU5" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BV5" s="15">
         <v>2</v>
@@ -3052,10 +3298,10 @@
         <v>4</v>
       </c>
       <c r="BX5" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BY5" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BZ5" s="15">
         <v>0</v>
@@ -3063,10 +3309,10 @@
     </row>
     <row r="6" spans="1:79">
       <c r="A6" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>3</v>
@@ -3201,7 +3447,7 @@
         <v>9</v>
       </c>
       <c r="AV6" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AW6" s="15">
         <v>3</v>
@@ -3219,7 +3465,7 @@
         <v>2</v>
       </c>
       <c r="BB6" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BC6" s="15">
         <v>9</v>
@@ -3237,16 +3483,16 @@
         <v>3</v>
       </c>
       <c r="BH6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BI6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BJ6" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BK6" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BL6" s="15">
         <v>0</v>
@@ -3255,19 +3501,19 @@
         <v>0</v>
       </c>
       <c r="BN6" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BO6" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BP6" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BQ6" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BR6" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BS6" s="15">
         <v>4</v>
@@ -3276,7 +3522,7 @@
         <v>5</v>
       </c>
       <c r="BU6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BV6" s="15">
         <v>6</v>
@@ -3288,18 +3534,18 @@
         <v>3</v>
       </c>
       <c r="BY6" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BZ6" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:79">
       <c r="A7" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>3</v>
@@ -3431,25 +3677,25 @@
         <v>1</v>
       </c>
       <c r="AU7" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AV7" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AW7" s="15">
         <v>2</v>
       </c>
       <c r="AX7" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AY7" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AZ7" s="15">
         <v>2</v>
       </c>
       <c r="BA7" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BB7" s="15">
         <v>8</v>
@@ -3458,7 +3704,7 @@
         <v>5</v>
       </c>
       <c r="BD7" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BE7" s="15">
         <v>2</v>
@@ -3470,7 +3716,7 @@
         <v>6</v>
       </c>
       <c r="BH7" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BI7" s="15">
         <v>8</v>
@@ -3482,7 +3728,7 @@
         <v>9</v>
       </c>
       <c r="BL7" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BM7" s="15">
         <v>5</v>
@@ -3494,13 +3740,13 @@
         <v>1</v>
       </c>
       <c r="BP7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="BQ7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BR7" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="BQ7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="BR7" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="BS7" s="15">
         <v>5</v>
@@ -3521,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="BY7" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BZ7" s="15">
         <v>6</v>
@@ -3529,10 +3775,10 @@
     </row>
     <row r="8" spans="1:79">
       <c r="A8" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>3</v>
@@ -3670,28 +3916,28 @@
         <v>1</v>
       </c>
       <c r="AW8" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AX8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AY8" s="15">
         <v>1</v>
       </c>
       <c r="AZ8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BA8" s="15">
         <v>8</v>
       </c>
       <c r="BB8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BC8" s="15">
         <v>3</v>
       </c>
       <c r="BD8" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BE8" s="15">
         <v>4</v>
@@ -3700,13 +3946,13 @@
         <v>9</v>
       </c>
       <c r="BG8" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BH8" s="15">
         <v>8</v>
       </c>
       <c r="BI8" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BJ8" s="15">
         <v>9</v>
@@ -3718,10 +3964,10 @@
         <v>9</v>
       </c>
       <c r="BM8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BN8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BO8" s="15">
         <v>4</v>
@@ -3733,25 +3979,25 @@
         <v>6</v>
       </c>
       <c r="BR8" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BS8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="BT8" s="15">
+        <v>5</v>
+      </c>
+      <c r="BU8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="BT8" s="15">
-        <v>5</v>
-      </c>
-      <c r="BU8" s="15" t="s">
-        <v>34</v>
-      </c>
       <c r="BV8" s="15">
         <v>0</v>
       </c>
       <c r="BW8" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BX8" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BY8" s="15">
         <v>9</v>
@@ -3762,10 +4008,10 @@
     </row>
     <row r="9" spans="1:79">
       <c r="A9" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>3</v>
@@ -3900,16 +4146,16 @@
         <v>9</v>
       </c>
       <c r="AV9" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AW9" s="15">
         <v>5</v>
       </c>
       <c r="AX9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY9" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="AY9" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="AZ9" s="15">
         <v>3</v>
@@ -3924,7 +4170,7 @@
         <v>6</v>
       </c>
       <c r="BD9" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BE9" s="15">
         <v>3</v>
@@ -3936,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="BH9" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BI9" s="15">
         <v>6</v>
@@ -3945,7 +4191,7 @@
         <v>5</v>
       </c>
       <c r="BK9" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BL9" s="15">
         <v>6</v>
@@ -3957,13 +4203,13 @@
         <v>7</v>
       </c>
       <c r="BO9" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BP9" s="15">
         <v>2</v>
       </c>
       <c r="BQ9" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BR9" s="15">
         <v>6</v>
@@ -3975,7 +4221,7 @@
         <v>7</v>
       </c>
       <c r="BU9" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BV9" s="15">
         <v>7</v>
@@ -3990,15 +4236,15 @@
         <v>1</v>
       </c>
       <c r="BZ9" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:79">
       <c r="A13" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>3</v>
@@ -4133,7 +4379,7 @@
         <v>3</v>
       </c>
       <c r="AV13" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AW13" s="15">
         <v>6</v>
@@ -4142,10 +4388,10 @@
         <v>1</v>
       </c>
       <c r="AY13" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AZ13" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BA13" s="15">
         <v>5</v>
@@ -4157,13 +4403,13 @@
         <v>4</v>
       </c>
       <c r="BD13" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BE13" s="15">
         <v>6</v>
       </c>
       <c r="BF13" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BG13" s="15">
         <v>9</v>
@@ -4184,7 +4430,7 @@
         <v>1</v>
       </c>
       <c r="BM13" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BN13" s="15">
         <v>7</v>
@@ -4199,7 +4445,7 @@
         <v>9</v>
       </c>
       <c r="BR13" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BS13" s="15">
         <v>4</v>
@@ -4208,7 +4454,7 @@
         <v>5</v>
       </c>
       <c r="BU13" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BV13" s="15">
         <v>5</v>
@@ -4217,7 +4463,7 @@
         <v>9</v>
       </c>
       <c r="BX13" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BY13" s="15">
         <v>9</v>
@@ -4228,10 +4474,10 @@
     </row>
     <row r="14" spans="1:79">
       <c r="A14" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>3</v>
@@ -4378,13 +4624,13 @@
         <v>9</v>
       </c>
       <c r="AZ14" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BA14" s="15">
         <v>5</v>
       </c>
       <c r="BB14" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BC14" s="15">
         <v>4</v>
@@ -4396,7 +4642,7 @@
         <v>5</v>
       </c>
       <c r="BF14" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BG14" s="15">
         <v>1</v>
@@ -4411,7 +4657,7 @@
         <v>4</v>
       </c>
       <c r="BK14" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BL14" s="15">
         <v>2</v>
@@ -4420,22 +4666,22 @@
         <v>4</v>
       </c>
       <c r="BN14" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BO14" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BP14" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BQ14" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BR14" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BS14" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BT14" s="15">
         <v>8</v>
@@ -4453,18 +4699,18 @@
         <v>7</v>
       </c>
       <c r="BY14" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BZ14" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:79">
       <c r="A15" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>3</v>
@@ -4602,13 +4848,13 @@
         <v>1</v>
       </c>
       <c r="AW15" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AX15" s="15">
         <v>2</v>
       </c>
       <c r="AY15" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AZ15" s="15">
         <v>1</v>
@@ -4620,35 +4866,35 @@
         <v>3</v>
       </c>
       <c r="BC15" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BD15" s="15">
         <v>1</v>
       </c>
       <c r="BE15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BF15" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG15" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="BF15" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BG15" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BH15" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="BI15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BJ15" s="15">
+        <v>2</v>
+      </c>
+      <c r="BK15" s="15">
+        <v>8</v>
+      </c>
+      <c r="BL15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="BJ15" s="15">
-        <v>2</v>
-      </c>
-      <c r="BK15" s="15">
-        <v>8</v>
-      </c>
-      <c r="BL15" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="BM15" s="15">
         <v>8</v>
       </c>
@@ -4662,42 +4908,42 @@
         <v>4</v>
       </c>
       <c r="BQ15" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BR15" s="15">
         <v>5</v>
       </c>
       <c r="BS15" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BT15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BU15" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BV15" s="15">
         <v>2</v>
       </c>
       <c r="BW15" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BX15" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BY15" s="15">
         <v>7</v>
       </c>
       <c r="BZ15" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:79">
       <c r="A16" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>3</v>
@@ -4832,7 +5078,7 @@
         <v>5</v>
       </c>
       <c r="AV16" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AW16" s="15">
         <v>9</v>
@@ -4844,7 +5090,7 @@
         <v>4</v>
       </c>
       <c r="AZ16" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BA16" s="15">
         <v>4</v>
@@ -4853,19 +5099,19 @@
         <v>5</v>
       </c>
       <c r="BC16" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BD16" s="15">
         <v>7</v>
       </c>
       <c r="BE16" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BF16" s="15">
         <v>2</v>
       </c>
       <c r="BG16" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BH16" s="15">
         <v>4</v>
@@ -4874,13 +5120,13 @@
         <v>6</v>
       </c>
       <c r="BJ16" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BK16" s="15">
         <v>4</v>
       </c>
       <c r="BL16" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BM16" s="15">
         <v>3</v>
@@ -4892,7 +5138,7 @@
         <v>3</v>
       </c>
       <c r="BP16" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BQ16" s="15">
         <v>4</v>
@@ -4901,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="BS16" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BT16" s="15">
         <v>6</v>
@@ -4916,7 +5162,7 @@
         <v>5</v>
       </c>
       <c r="BX16" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BY16" s="15">
         <v>4</v>
@@ -4927,10 +5173,10 @@
     </row>
     <row r="17" spans="1:78">
       <c r="A17" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>3</v>
@@ -5062,7 +5308,7 @@
         <v>9</v>
       </c>
       <c r="AU17" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AV17" s="15">
         <v>6</v>
@@ -5077,13 +5323,13 @@
         <v>3</v>
       </c>
       <c r="AZ17" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BA17" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BB17" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BC17" s="15">
         <v>6</v>
@@ -5092,7 +5338,7 @@
         <v>4</v>
       </c>
       <c r="BE17" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BF17" s="15">
         <v>0</v>
@@ -5104,7 +5350,7 @@
         <v>9</v>
       </c>
       <c r="BI17" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BJ17" s="15">
         <v>5</v>
@@ -5116,7 +5362,7 @@
         <v>8</v>
       </c>
       <c r="BM17" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BN17" s="15">
         <v>9</v>
@@ -5125,42 +5371,42 @@
         <v>3</v>
       </c>
       <c r="BP17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BQ17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BR17" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="BQ17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="BR17" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="BS17" s="15">
         <v>5</v>
       </c>
       <c r="BT17" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BU17" s="15">
         <v>6</v>
       </c>
       <c r="BV17" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BW17" s="15">
         <v>4</v>
       </c>
       <c r="BX17" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BY17" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BZ17" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:78">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>3</v>
@@ -5296,28 +5542,28 @@
         <v>2</v>
       </c>
       <c r="AW21" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AX21" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AY21" s="15">
         <v>8</v>
       </c>
       <c r="AZ21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA21" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="BA21" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB21" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="BC21" s="15">
         <v>4</v>
       </c>
       <c r="BD21" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BE21" s="15">
         <v>7</v>
@@ -5326,7 +5572,7 @@
         <v>3</v>
       </c>
       <c r="BG21" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BH21" s="15">
         <v>9</v>
@@ -5335,7 +5581,7 @@
         <v>8</v>
       </c>
       <c r="BJ21" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BK21" s="15">
         <v>6</v>
@@ -5374,7 +5620,7 @@
         <v>6</v>
       </c>
       <c r="BW21" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BX21" s="15">
         <v>2</v>
@@ -5388,34 +5634,34 @@
     </row>
     <row r="22" spans="1:78">
       <c r="A22" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="16"/>
     </row>
     <row r="24" spans="1:78">
       <c r="A24" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:78">
       <c r="A25" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:78">
       <c r="A26" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:78">
       <c r="A27" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AH27" s="16"/>
     </row>
     <row r="28" spans="1:78">
       <c r="A28" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AO28" s="16"/>
     </row>

</xml_diff>